<commit_message>
Adding Unit 1.3 solutions
</commit_message>
<xml_diff>
--- a/01-Class-Activities/Mon-Wed-Class/01-Excel/3/Activities/08-Ins_MovingAverages/Solved/MovingAverages.xlsx
+++ b/01-Class-Activities/Mon-Wed-Class/01-Excel/3/Activities/08-Ins_MovingAverages/Solved/MovingAverages.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacob\OneDrive\Documents\WorkAndSchool\TeachingAssistant\DataViz\DataViz-Lesson-Plans\01-Lesson-Plans\01-Excel\3\Activities\08-Ins_MovingAverages\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\98452\Documents\GitHub\GWU-ARL-DATA-PT-09-2019-U-C\01-Class-Activities\Tue-Thurs-Class\01-Excel\3\Activities\08-Ins_MovingAverages\Solved\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="51B984A3CC64C4236FA77ED876DEF10FB53764FF" xr6:coauthVersionLast="21" xr6:coauthVersionMax="21" xr10:uidLastSave="{50C89576-D7D7-416C-ABD6-84E385541CF0}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="12780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="12780"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -99,7 +98,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{D49F0EF7-EFF3-4B63-86D0-01C41125D719}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -113,6 +112,1180 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Moving Averages Example</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Period</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$1:$M$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-CC84-47B7-A40E-BA4FD228BF79}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Actual</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$M$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>540</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>380</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>870</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>950</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-CC84-47B7-A40E-BA4FD228BF79}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Interval(2)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$3:$M$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>195</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>390</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>375</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>295</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>495</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>560</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>675</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>725</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-CC84-47B7-A40E-BA4FD228BF79}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Interval(4)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$4:$M$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>262.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>285</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>342.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>312.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>395</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>405</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>585</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>680</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>700</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-CC84-47B7-A40E-BA4FD228BF79}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="2004499968"/>
+        <c:axId val="2004503296"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2004499968"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2004503296"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2004503296"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2004499968"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -411,21 +1584,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:M4"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.73046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="13" width="5.59765625" customWidth="1"/>
-    <col min="14" max="14" width="4.86328125" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="13" width="5.5703125" customWidth="1"/>
+    <col min="14" max="14" width="4.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -466,7 +1637,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -507,17 +1678,110 @@
         <v>950</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
+      <c r="B3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:M3" si="0">AVERAGE(B2:C2)</f>
+        <v>135</v>
+      </c>
+      <c r="D3">
+        <f t="shared" si="0"/>
+        <v>195</v>
+      </c>
+      <c r="E3">
+        <f t="shared" si="0"/>
+        <v>390</v>
+      </c>
+      <c r="F3">
+        <f t="shared" si="0"/>
+        <v>375</v>
+      </c>
+      <c r="G3">
+        <f t="shared" si="0"/>
+        <v>295</v>
+      </c>
+      <c r="H3">
+        <f t="shared" si="0"/>
+        <v>250</v>
+      </c>
+      <c r="I3">
+        <f t="shared" si="0"/>
+        <v>495</v>
+      </c>
+      <c r="J3">
+        <f t="shared" si="0"/>
+        <v>560</v>
+      </c>
+      <c r="K3">
+        <f t="shared" si="0"/>
+        <v>675</v>
+      </c>
+      <c r="L3">
+        <f t="shared" si="0"/>
+        <v>800</v>
+      </c>
+      <c r="M3">
+        <f t="shared" si="0"/>
+        <v>725</v>
+      </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
+      </c>
+      <c r="B4" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C4" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D4" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4:M4" si="1">AVERAGE(B2:E2)</f>
+        <v>262.5</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>285</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="1"/>
+        <v>342.5</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="1"/>
+        <v>312.5</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="1"/>
+        <v>395</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="1"/>
+        <v>405</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="1"/>
+        <v>585</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="1"/>
+        <v>680</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="1"/>
+        <v>700</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>